<commit_message>
* added PD_direction2 function in gui.m ... but still it is not good. flipping happens.
</commit_message>
<xml_diff>
--- a/TPro/input/input_video_control.xlsx
+++ b/TPro/input/input_video_control.xlsx
@@ -63,7 +63,7 @@
     <t>Step</t>
   </si>
   <si>
-    <t>LearningDemoX1.avi</t>
+    <t>cut_Video_14.avi</t>
   </si>
 </sst>
 </file>
@@ -461,16 +461,16 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>1000</v>
+        <v>1184</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I2">
         <v>0.6</v>
@@ -485,13 +485,13 @@
         <v>2000</v>
       </c>
       <c r="M2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="P2">
         <v>1</v>

</xml_diff>